<commit_message>
Correct type in example data
</commit_message>
<xml_diff>
--- a/exampleData/Example-1.xlsx
+++ b/exampleData/Example-1.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">Date of Birth</t>
   </si>
   <si>
-    <t xml:space="preserve">Adress Line 1</t>
+    <t xml:space="preserve">Address Line 1</t>
   </si>
   <si>
     <t xml:space="preserve">Postcode</t>
@@ -209,6 +209,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -227,22 +228,25 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -292,24 +296,28 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -321,7 +329,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Accent 1" xfId="20"/>
+    <cellStyle name="Accent 1 1" xfId="20"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -440,235 +448,235 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="4" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update exampleData to include int field
</commit_message>
<xml_diff>
--- a/exampleData/Example-1.xlsx
+++ b/exampleData/Example-1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
   <si>
     <t xml:space="preserve">Forename</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t xml:space="preserve">Active</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Credit Score</t>
   </si>
   <si>
     <t xml:space="preserve">John</t>
@@ -200,9 +203,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -300,7 +304,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -318,6 +322,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -445,10 +453,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -458,6 +466,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -479,205 +488,238 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="4" t="s">
         <v>11</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>234</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="4" t="s">
         <v>17</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>405</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>11</v>
+        <v>23</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>654</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>17</v>
+        <v>28</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>753</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>11</v>
+        <v>33</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>572</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>17</v>
+        <v>38</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>357</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>11</v>
+        <v>43</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>346</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>17</v>
+        <v>48</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>459</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>11</v>
+        <v>53</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>625</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>17</v>
+        <v>58</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>